<commit_message>
feat: Update the "Besk cup" game results with the approved controversials.
</commit_message>
<xml_diff>
--- a/src/main/resources/tournament-tours-9416-15-Sep-2023.xlsx
+++ b/src/main/resources/tournament-tours-9416-15-Sep-2023.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
   <si>
     <t>Team ID</t>
   </si>
@@ -78,18 +77,6 @@
   </si>
   <si>
     <t>ZERO Yard</t>
-  </si>
-  <si>
-    <t>фиговый листок</t>
-  </si>
-  <si>
-    <t>фиговый лист</t>
-  </si>
-  <si>
-    <t>his imagination</t>
-  </si>
-  <si>
-    <t>His Intelligence</t>
   </si>
   <si>
     <t>Hi
@@ -140,7 +127,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,7 +136,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,17 +169,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -492,16 +488,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="16" width="5.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="16" width="3.5703125" style="1" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -574,7 +572,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -988,8 +986,8 @@
       <c r="K11" s="1">
         <v>0</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>26</v>
+      <c r="L11" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="M11" s="1">
         <v>0</v>
@@ -1185,8 +1183,8 @@
       <c r="J16" s="1">
         <v>1</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>24</v>
+      <c r="K16" s="6">
+        <v>1</v>
       </c>
       <c r="L16" s="1">
         <v>1</v>
@@ -1235,8 +1233,8 @@
       <c r="J17" s="1">
         <v>1</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>23</v>
+      <c r="K17" s="6">
+        <v>1</v>
       </c>
       <c r="L17" s="1">
         <v>0</v>
@@ -1285,8 +1283,8 @@
       <c r="J18" s="1">
         <v>1</v>
       </c>
-      <c r="K18" s="7" t="s">
-        <v>25</v>
+      <c r="K18" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="L18" s="1">
         <v>0</v>
@@ -1382,11 +1380,11 @@
       <c r="I20" s="1">
         <v>0</v>
       </c>
-      <c r="J20" s="4" t="s">
-        <v>22</v>
+      <c r="J20" s="6">
+        <v>1</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
@@ -1535,8 +1533,8 @@
       <c r="J23" s="1">
         <v>1</v>
       </c>
-      <c r="K23" s="4" t="s">
-        <v>23</v>
+      <c r="K23" s="6">
+        <v>1</v>
       </c>
       <c r="L23" s="1">
         <v>0</v>
@@ -1582,8 +1580,8 @@
       <c r="I24" s="1">
         <v>0</v>
       </c>
-      <c r="J24" s="4" t="s">
-        <v>21</v>
+      <c r="J24" s="6">
+        <v>1</v>
       </c>
       <c r="K24" s="1">
         <v>0</v>
@@ -1798,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="P29" s="1">
         <v>0</v>

</xml_diff>